<commit_message>
modify syn car logic.
</commit_message>
<xml_diff>
--- a/docs/20180512映射地址集.xlsx
+++ b/docs/20180512映射地址集.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Desktop\ProductionLineMonitor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F7C27F73-B07F-48BE-A30B-E5363745716D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{086EEA17-5B00-41A4-A6F6-332B4DE27A6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7330,12 +7330,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="90">

</xml_diff>